<commit_message>
App_9 file for scope 2 and scope 1
</commit_message>
<xml_diff>
--- a/GWP.xlsx
+++ b/GWP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RituGothwal\Stok LLC\Python Scripts\Emission factor tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebs1-my.sharepoint.com/personal/ritu_stok_com/Documents/Ritu/Python Scripts/Carbon_team_Scripts/Emission_factor_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9B9D2FB-DC17-4E60-8A69-F635E0BBB45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{B9B9D2FB-DC17-4E60-8A69-F635E0BBB45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73A042C4-0918-4503-BD75-73641B12AAAF}"/>
   <bookViews>
-    <workbookView xWindow="-26088" yWindow="1728" windowWidth="23040" windowHeight="12120" xr2:uid="{F347CA65-B804-4495-9E3F-192DE944BC12}"/>
+    <workbookView xWindow="30612" yWindow="-432" windowWidth="30936" windowHeight="16776" xr2:uid="{F347CA65-B804-4495-9E3F-192DE944BC12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>CO2</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>CFC-115</t>
+  </si>
+  <si>
+    <t>AR6</t>
   </si>
 </sst>
 </file>
@@ -128,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -151,16 +154,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3EF495D-F045-408B-A762-BECCDE976B7E}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +525,7 @@
     <col min="4" max="4" width="7.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -522,8 +538,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -536,8 +555,11 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -550,8 +572,11 @@
       <c r="D3" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -564,8 +589,11 @@
       <c r="D4" s="2">
         <v>265</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -578,8 +606,9 @@
       <c r="D5" s="3">
         <v>4660</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -593,7 +622,7 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -605,7 +634,7 @@
         <v>13900</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -619,7 +648,7 @@
         <v>5820</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -631,7 +660,7 @@
         <v>8590</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>